<commit_message>
[FIX] xlsx: import data validation rules with formula
Data validations rules with formulas were not correctly imported,
ad they are not prefixed by "=" in the xlsx, but should be in
o-spreadsheet.

Task: 5062253
</commit_message>
<xml_diff>
--- a/tests/__xlsx__/xlsx_demo_data.xlsx
+++ b/tests/__xlsx__/xlsx_demo_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Odoo\spreadsheet\tests\__xlsx__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDCA15CC-80FD-451D-A815-3D3194402FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C54EF9F-11D5-4F87-92EE-DAA682A5CDBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1755" windowWidth="29040" windowHeight="18240" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
   </externalReferences>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId16"/>
+    <pivotCache cacheId="0" r:id="rId16"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="442">
   <si>
     <t>CF =42</t>
   </si>
@@ -1379,6 +1379,9 @@
   </si>
   <si>
     <t>CF with formulas</t>
+  </si>
+  <si>
+    <t>Decimal with formula</t>
   </si>
 </sst>
 </file>
@@ -1558,7 +1561,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="30">
+  <fills count="29">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1739,14 +1742,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="36">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -2100,55 +2097,6 @@
         <color rgb="FF000000"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
@@ -2187,7 +2135,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2368,23 +2316,13 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="29" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="20" fontId="0" fillId="29" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="29" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="29" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2406,6 +2344,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -2413,13 +2354,6 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{1493241F-B85D-4F84-BBA0-86191B8FD032}"/>
   </cellStyles>
   <dxfs count="47">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2458,6 +2392,13 @@
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -7912,7 +7853,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="C3:L21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -8529,7 +8470,7 @@
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="117" t="s">
+      <c r="G1" s="107" t="s">
         <v>1</v>
       </c>
     </row>
@@ -8540,26 +8481,26 @@
       <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="117">
+      <c r="G2" s="107">
         <v>5</v>
       </c>
-      <c r="H2" s="118" t="s">
+      <c r="H2" s="108" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="119"/>
+      <c r="I2" s="109"/>
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="117">
+      <c r="G3" s="107">
         <v>8</v>
       </c>
-      <c r="H3" s="119"/>
-      <c r="I3" s="119"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="109"/>
       <c r="J3" s="5"/>
-      <c r="K3" s="120">
+      <c r="K3" s="110">
         <v>5</v>
       </c>
       <c r="L3" s="6"/>
@@ -8568,94 +8509,94 @@
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="117">
+      <c r="C4" s="107">
         <v>12.4</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="117">
+      <c r="G4" s="107">
         <v>9</v>
       </c>
-      <c r="H4" s="119"/>
-      <c r="I4" s="119"/>
+      <c r="H4" s="109"/>
+      <c r="I4" s="109"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="121"/>
+      <c r="K4" s="111"/>
       <c r="L4" s="6"/>
     </row>
     <row r="5" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="117">
+      <c r="C5" s="107">
         <v>42</v>
       </c>
-      <c r="G5" s="117">
+      <c r="G5" s="107">
         <v>15</v>
       </c>
-      <c r="H5" s="119"/>
-      <c r="I5" s="119"/>
+      <c r="H5" s="109"/>
+      <c r="I5" s="109"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="121"/>
+      <c r="K5" s="111"/>
       <c r="L5" s="6"/>
     </row>
     <row r="6" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G6" s="117">
+      <c r="G6" s="107">
         <v>22</v>
       </c>
       <c r="J6" s="5"/>
-      <c r="K6" s="121"/>
+      <c r="K6" s="111"/>
       <c r="L6" s="6"/>
     </row>
     <row r="7" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="117">
+      <c r="C7" s="107">
         <v>3</v>
       </c>
       <c r="J7" s="5"/>
-      <c r="K7" s="121"/>
+      <c r="K7" s="111"/>
       <c r="L7" s="6"/>
     </row>
     <row r="8" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G8" s="117">
+      <c r="G8" s="107">
         <v>30</v>
       </c>
       <c r="J8" s="5"/>
-      <c r="K8" s="122"/>
+      <c r="K8" s="112"/>
       <c r="L8" s="6"/>
     </row>
     <row r="9" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="117">
+      <c r="C9" s="107">
         <f>SUM(C4:C5)</f>
         <v>54.4</v>
       </c>
       <c r="K9" s="10"/>
     </row>
     <row r="10" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="117">
+      <c r="C10" s="107">
         <f>SUM(C4:C7)</f>
         <v>57.4</v>
       </c>
-      <c r="D10" s="117" t="s">
+      <c r="D10" s="107" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="117">
+      <c r="C11" s="107">
         <f>-(3+C7*SUM(C4:C7))</f>
         <v>-175.2</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C12" s="117">
+      <c r="C12" s="107">
         <f>SUM(C9:C11)</f>
         <v>-63.399999999999991</v>
       </c>
-      <c r="D12" s="117" t="s">
+      <c r="D12" s="107" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G13" s="117">
+      <c r="G13" s="107">
         <f>A1+A2+A3+A4+A5+A6+A7+A8+A9+A10+A11+A12+A13+A14+A15+A16+A17+A18</f>
         <v>0</v>
       </c>
@@ -8664,29 +8605,29 @@
       <c r="B14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="117" t="str">
+      <c r="C14" s="107" t="str">
         <f ca="1">C14</f>
         <v>#CYCLE</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C15" s="117" t="s">
+      <c r="C15" s="107" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C16" s="117" t="str">
+      <c r="C16" s="107" t="str">
         <f>C15</f>
         <v>=(+</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C17" s="117" t="s">
+      <c r="C17" s="107" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C18" s="117" t="s">
+      <c r="C18" s="107" t="s">
         <v>14</v>
       </c>
     </row>
@@ -8725,10 +8666,10 @@
       <c r="C23" s="15">
         <v>0.43</v>
       </c>
-      <c r="H23" s="117">
+      <c r="H23" s="107">
         <v>0</v>
       </c>
-      <c r="I23" s="117">
+      <c r="I23" s="107">
         <v>0</v>
       </c>
     </row>
@@ -8736,10 +8677,10 @@
       <c r="C24" s="16">
         <v>10</v>
       </c>
-      <c r="H24" s="117">
-        <v>1</v>
-      </c>
-      <c r="I24" s="117">
+      <c r="H24" s="107">
+        <v>1</v>
+      </c>
+      <c r="I24" s="107">
         <v>1</v>
       </c>
     </row>
@@ -8747,165 +8688,165 @@
       <c r="C25" s="16">
         <v>10.122999999999999</v>
       </c>
-      <c r="H25" s="117">
+      <c r="H25" s="107">
         <v>2</v>
       </c>
-      <c r="I25" s="117">
+      <c r="I25" s="107">
         <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="117" t="s">
+      <c r="B26" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="117" t="s">
+      <c r="C26" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="H26" s="117">
+      <c r="H26" s="107">
         <v>3</v>
       </c>
-      <c r="I26" s="117">
+      <c r="I26" s="107">
         <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="117" t="s">
+      <c r="A27" s="107" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="117">
+      <c r="B27" s="107">
         <v>12</v>
       </c>
-      <c r="C27" s="117">
+      <c r="C27" s="107">
         <v>24</v>
       </c>
-      <c r="H27" s="117">
+      <c r="H27" s="107">
         <v>4</v>
       </c>
-      <c r="I27" s="117">
+      <c r="I27" s="107">
         <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="117" t="s">
+      <c r="A28" s="107" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="117">
+      <c r="B28" s="107">
         <v>48</v>
       </c>
-      <c r="C28" s="117">
+      <c r="C28" s="107">
         <v>12</v>
       </c>
-      <c r="H28" s="117">
+      <c r="H28" s="107">
         <v>5</v>
       </c>
-      <c r="I28" s="117">
+      <c r="I28" s="107">
         <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="117" t="s">
+      <c r="A29" s="107" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="117">
+      <c r="B29" s="107">
         <v>45</v>
       </c>
-      <c r="C29" s="117">
+      <c r="C29" s="107">
         <v>27</v>
       </c>
-      <c r="H29" s="117">
+      <c r="H29" s="107">
         <v>6</v>
       </c>
-      <c r="I29" s="117">
+      <c r="I29" s="107">
         <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="117" t="s">
+      <c r="A30" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="B30" s="117">
-        <v>1</v>
-      </c>
-      <c r="C30" s="117">
+      <c r="B30" s="107">
+        <v>1</v>
+      </c>
+      <c r="C30" s="107">
         <v>9</v>
       </c>
-      <c r="H30" s="117">
+      <c r="H30" s="107">
         <v>7</v>
       </c>
-      <c r="I30" s="117">
+      <c r="I30" s="107">
         <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="117" t="s">
+      <c r="A31" s="107" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="117">
+      <c r="B31" s="107">
         <v>25</v>
       </c>
-      <c r="C31" s="117">
+      <c r="C31" s="107">
         <v>45</v>
       </c>
-      <c r="H31" s="117">
+      <c r="H31" s="107">
         <v>8</v>
       </c>
-      <c r="I31" s="117">
+      <c r="I31" s="107">
         <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="117" t="s">
+      <c r="A32" s="107" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="117">
+      <c r="B32" s="107">
         <v>31</v>
       </c>
-      <c r="C32" s="117">
+      <c r="C32" s="107">
         <v>17</v>
       </c>
-      <c r="H32" s="117">
+      <c r="H32" s="107">
         <v>9</v>
       </c>
-      <c r="I32" s="117">
+      <c r="I32" s="107">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="117" t="s">
+      <c r="A33" s="107" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="117">
+      <c r="B33" s="107">
         <v>20</v>
       </c>
-      <c r="C33" s="117">
+      <c r="C33" s="107">
         <v>43</v>
       </c>
-      <c r="H33" s="117">
+      <c r="H33" s="107">
         <v>10</v>
       </c>
-      <c r="I33" s="117">
+      <c r="I33" s="107">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="117" t="s">
+      <c r="A34" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="117">
+      <c r="B34" s="107">
         <v>19</v>
       </c>
-      <c r="C34" s="117">
+      <c r="C34" s="107">
         <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="117" t="s">
+      <c r="A35" s="107" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="117">
+      <c r="B35" s="107">
         <v>16</v>
       </c>
-      <c r="C35" s="117">
+      <c r="C35" s="107">
         <v>16</v>
       </c>
     </row>
@@ -9025,10 +8966,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{025F2510-D243-4DA1-81DE-BBDDA9BC3681}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9038,184 +8979,203 @@
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
     <col min="8" max="8" width="20.28515625" customWidth="1"/>
     <col min="9" max="9" width="17.28515625" customWidth="1"/>
+    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="s">
+    <row r="1" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="104" t="s">
         <v>423</v>
       </c>
-      <c r="B1" s="115" t="s">
+      <c r="B1" s="105" t="s">
         <v>424</v>
       </c>
-      <c r="C1" s="115" t="s">
+      <c r="C1" s="105" t="s">
         <v>425</v>
       </c>
-      <c r="D1" s="115" t="s">
+      <c r="D1" s="105" t="s">
         <v>426</v>
       </c>
-      <c r="E1" s="115" t="s">
+      <c r="E1" s="105" t="s">
         <v>427</v>
       </c>
-      <c r="F1" s="115" t="s">
+      <c r="F1" s="105" t="s">
         <v>428</v>
       </c>
-      <c r="G1" s="115" t="s">
+      <c r="G1" s="105" t="s">
         <v>429</v>
       </c>
-      <c r="H1" s="115" t="s">
+      <c r="H1" s="105" t="s">
         <v>430</v>
       </c>
-      <c r="I1" s="116" t="s">
+      <c r="I1" s="106" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="104">
+      <c r="J1" s="114" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>4</v>
       </c>
-      <c r="B2" s="105">
+      <c r="B2">
         <v>99.5</v>
       </c>
-      <c r="C2" s="105">
-        <v>1</v>
-      </c>
-      <c r="D2" s="105" t="s">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>432</v>
       </c>
-      <c r="E2" s="106">
+      <c r="E2">
         <v>45575</v>
       </c>
-      <c r="F2" s="107">
+      <c r="F2">
         <v>0.64583333333333337</v>
       </c>
-      <c r="G2" s="107" t="s">
+      <c r="G2" t="s">
         <v>433</v>
       </c>
-      <c r="H2" s="106">
+      <c r="H2">
         <v>45292</v>
       </c>
-      <c r="I2" s="108">
+      <c r="I2">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="104">
+      <c r="J2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>3</v>
       </c>
-      <c r="B3" s="105">
+      <c r="B3">
         <v>40</v>
       </c>
-      <c r="C3" s="105">
+      <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3" s="105" t="s">
+      <c r="D3" t="s">
         <v>434</v>
       </c>
-      <c r="E3" s="106">
+      <c r="E3">
         <v>45576</v>
       </c>
-      <c r="F3" s="107">
+      <c r="F3">
         <v>0.57638888888888884</v>
       </c>
-      <c r="G3" s="107" t="s">
+      <c r="G3" t="s">
         <v>435</v>
       </c>
-      <c r="H3" s="106">
+      <c r="H3">
         <v>45231</v>
       </c>
-      <c r="I3" s="108" t="s">
+      <c r="I3" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="104">
+      <c r="J3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>9</v>
       </c>
-      <c r="B4" s="105">
+      <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4" s="105">
+      <c r="C4">
         <v>3</v>
       </c>
-      <c r="D4" s="105" t="s">
+      <c r="D4" t="s">
         <v>436</v>
       </c>
-      <c r="E4" s="106">
+      <c r="E4">
         <v>45574</v>
       </c>
-      <c r="F4" s="107">
+      <c r="F4">
         <v>0.73958333333333337</v>
       </c>
-      <c r="G4" s="107" t="s">
+      <c r="G4" t="s">
         <v>437</v>
       </c>
-      <c r="H4" s="106">
+      <c r="H4">
         <v>45325</v>
       </c>
-      <c r="I4" s="108">
+      <c r="I4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="104">
+      <c r="J4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>5</v>
       </c>
-      <c r="B5" s="105">
+      <c r="B5">
         <v>120</v>
       </c>
-      <c r="C5" s="105">
+      <c r="C5">
         <v>4</v>
       </c>
-      <c r="D5" s="105" t="s">
+      <c r="D5" t="s">
         <v>434</v>
       </c>
-      <c r="E5" s="106">
+      <c r="E5">
         <v>45573</v>
       </c>
-      <c r="F5" s="107">
+      <c r="F5">
         <v>0.66666666666666663</v>
       </c>
-      <c r="G5" s="105" t="s">
+      <c r="G5" t="s">
         <v>438</v>
       </c>
-      <c r="H5" s="106">
+      <c r="H5">
         <v>45084</v>
       </c>
-      <c r="I5" s="108">
+      <c r="I5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="109">
+      <c r="J5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>7</v>
       </c>
-      <c r="B6" s="110">
+      <c r="B6">
         <v>12</v>
       </c>
-      <c r="C6" s="110">
+      <c r="C6">
         <v>5</v>
       </c>
-      <c r="D6" s="110" t="s">
+      <c r="D6" t="s">
         <v>436</v>
       </c>
-      <c r="E6" s="111">
+      <c r="E6">
         <v>45566</v>
       </c>
-      <c r="F6" s="112">
+      <c r="F6">
         <v>0.5229166666666667</v>
       </c>
-      <c r="G6" s="110" t="s">
+      <c r="G6" t="s">
         <v>439</v>
       </c>
-      <c r="H6" s="111">
+      <c r="H6">
         <v>45420</v>
       </c>
-      <c r="I6" s="113" t="s">
+      <c r="I6" t="s">
         <v>438</v>
       </c>
+      <c r="J6">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="9">
+  <dataValidations count="10">
     <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A6" xr:uid="{B9309757-E2F4-49A1-880B-2F47F04364D6}">
       <formula1>1</formula1>
       <formula2>5</formula2>
@@ -9247,6 +9207,10 @@
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D6" xr:uid="{1E18A174-B5CF-4015-B7DC-F1491351E054}">
       <formula1>"option1,option2,option3"</formula1>
     </dataValidation>
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J6" xr:uid="{B2C1C92E-719F-4115-9CD6-F9CF0931A2A1}">
+      <formula1>$A$2</formula1>
+      <formula2>2+10</formula2>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9269,16 +9233,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="107" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="117" t="s">
+      <c r="B1" s="107" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="117" t="s">
+      <c r="C1" s="107" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="117" t="s">
+      <c r="D1" s="107" t="s">
         <v>34</v>
       </c>
       <c r="G1" s="17" t="s">
@@ -9296,7 +9260,7 @@
       <c r="K1" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="117">
+      <c r="N1" s="107">
         <v>0.1</v>
       </c>
       <c r="P1" s="17" t="s">
@@ -9304,36 +9268,36 @@
       </c>
     </row>
     <row r="2" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="117" t="s">
+      <c r="A2" s="107" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="117">
+      <c r="B2" s="107">
         <f>ABS(-5.5)</f>
         <v>5.5</v>
       </c>
-      <c r="C2" s="117">
+      <c r="C2" s="107">
         <v>5.5</v>
       </c>
-      <c r="D2" s="117">
+      <c r="D2" s="107">
         <f t="shared" ref="D2:D33" si="0">IF(B2=C2,1,0)</f>
         <v>1</v>
       </c>
-      <c r="G2" s="117" t="s">
+      <c r="G2" s="107" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="117">
+      <c r="H2" s="107">
         <v>26</v>
       </c>
-      <c r="I2" s="117">
+      <c r="I2" s="107">
         <v>1204.7</v>
       </c>
-      <c r="J2" s="117">
+      <c r="J2" s="107">
         <v>25618</v>
       </c>
-      <c r="K2" s="117">
+      <c r="K2" s="107">
         <v>5</v>
       </c>
-      <c r="N2" s="117">
+      <c r="N2" s="107">
         <v>0.2</v>
       </c>
       <c r="P2">
@@ -9350,36 +9314,36 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="117" t="s">
+      <c r="A3" s="107" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="117">
+      <c r="B3" s="107">
         <f>ACOS(1)</f>
         <v>0</v>
       </c>
-      <c r="C3" s="117">
+      <c r="C3" s="107">
         <v>0</v>
       </c>
-      <c r="D3" s="117">
+      <c r="D3" s="107">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G3" s="117" t="s">
+      <c r="G3" s="107" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="117">
+      <c r="H3" s="107">
         <v>13</v>
       </c>
-      <c r="I3" s="117">
+      <c r="I3" s="107">
         <v>500.9</v>
       </c>
-      <c r="J3" s="117">
+      <c r="J3" s="107">
         <v>23000</v>
       </c>
-      <c r="K3" s="117">
+      <c r="K3" s="107">
         <v>7</v>
       </c>
-      <c r="N3" s="117">
+      <c r="N3" s="107">
         <v>0.4</v>
       </c>
       <c r="P3">
@@ -9396,36 +9360,36 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="117" t="s">
+      <c r="A4" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="117">
+      <c r="B4" s="107">
         <f>ROUND(ACOSH(2),5)</f>
         <v>1.3169599999999999</v>
       </c>
-      <c r="C4" s="117">
+      <c r="C4" s="107">
         <v>1.3169599999999999</v>
       </c>
-      <c r="D4" s="117">
+      <c r="D4" s="107">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G4" s="117" t="s">
+      <c r="G4" s="107" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="117">
+      <c r="H4" s="107">
         <v>26</v>
       </c>
-      <c r="I4" s="117">
+      <c r="I4" s="107">
         <v>252.4</v>
       </c>
-      <c r="J4" s="117">
+      <c r="J4" s="107">
         <v>110120.5</v>
       </c>
-      <c r="K4" s="117">
+      <c r="K4" s="107">
         <v>3</v>
       </c>
-      <c r="N4" s="117">
+      <c r="N4" s="107">
         <v>0.5</v>
       </c>
       <c r="P4">
@@ -9442,36 +9406,36 @@
       </c>
     </row>
     <row r="5" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="117" t="s">
+      <c r="A5" s="107" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="117">
+      <c r="B5" s="107">
         <f>ROUND(_xlfn.ACOT(1),5)</f>
         <v>0.78539999999999999</v>
       </c>
-      <c r="C5" s="117">
+      <c r="C5" s="107">
         <v>0.78539999999999999</v>
       </c>
-      <c r="D5" s="117">
+      <c r="D5" s="107">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G5" s="117" t="s">
+      <c r="G5" s="107" t="s">
         <v>48</v>
       </c>
-      <c r="H5" s="117">
+      <c r="H5" s="107">
         <v>42</v>
       </c>
-      <c r="I5" s="117">
+      <c r="I5" s="107">
         <v>4701.3</v>
       </c>
-      <c r="J5" s="117">
+      <c r="J5" s="107">
         <v>50024</v>
       </c>
-      <c r="K5" s="117">
+      <c r="K5" s="107">
         <v>4</v>
       </c>
-      <c r="N5" s="117">
+      <c r="N5" s="107">
         <v>0.6</v>
       </c>
       <c r="P5">
@@ -9488,36 +9452,36 @@
       </c>
     </row>
     <row r="6" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="117" t="s">
+      <c r="A6" s="107" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="117">
+      <c r="B6" s="107">
         <f>ROUND(_xlfn.ACOTH(2),5)</f>
         <v>0.54930999999999996</v>
       </c>
-      <c r="C6" s="117">
+      <c r="C6" s="107">
         <v>0.54930999999999996</v>
       </c>
-      <c r="D6" s="117">
+      <c r="D6" s="107">
         <f>IF(B6=C6,1,0)</f>
         <v>1</v>
       </c>
-      <c r="G6" s="117" t="s">
+      <c r="G6" s="107" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="117">
+      <c r="H6" s="107">
         <v>9</v>
       </c>
-      <c r="I6" s="117">
+      <c r="I6" s="107">
         <v>12.1</v>
       </c>
-      <c r="J6" s="117">
+      <c r="J6" s="107">
         <v>2</v>
       </c>
-      <c r="K6" s="117">
+      <c r="K6" s="107">
         <v>1000</v>
       </c>
-      <c r="N6" s="117" t="s">
+      <c r="N6" s="107" t="s">
         <v>51</v>
       </c>
       <c r="P6">
@@ -9534,151 +9498,151 @@
       </c>
     </row>
     <row r="7" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="117" t="s">
+      <c r="A7" s="107" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="117" t="b">
+      <c r="B7" s="107" t="b">
         <f>AND(TRUE,TRUE)</f>
         <v>1</v>
       </c>
-      <c r="C7" s="117" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" s="117">
+      <c r="C7" s="107" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="107">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G7" s="117" t="s">
+      <c r="G7" s="107" t="s">
         <v>53</v>
       </c>
-      <c r="H7" s="117">
+      <c r="H7" s="107">
         <v>27</v>
       </c>
-      <c r="I7" s="117">
+      <c r="I7" s="107">
         <v>4000</v>
       </c>
-      <c r="J7" s="117">
+      <c r="J7" s="107">
         <v>189576</v>
       </c>
-      <c r="K7" s="117">
+      <c r="K7" s="107">
         <v>2</v>
       </c>
-      <c r="N7" s="117" t="b">
+      <c r="N7" s="107" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="117" t="s">
+      <c r="A8" s="107" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="117">
+      <c r="B8" s="107">
         <f>ROUND(ASIN(0.5),5)</f>
         <v>0.52359999999999995</v>
       </c>
-      <c r="C8" s="117">
+      <c r="C8" s="107">
         <v>0.52359999999999995</v>
       </c>
-      <c r="D8" s="117">
+      <c r="D8" s="107">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G8" s="117" t="s">
+      <c r="G8" s="107" t="s">
         <v>55</v>
       </c>
-      <c r="H8" s="117">
+      <c r="H8" s="107">
         <v>30</v>
       </c>
-      <c r="I8" s="117">
+      <c r="I8" s="107">
         <v>12052</v>
       </c>
-      <c r="J8" s="117">
+      <c r="J8" s="107">
         <v>256018</v>
       </c>
-      <c r="K8" s="117">
-        <v>1</v>
-      </c>
-      <c r="N8" s="117" t="b">
+      <c r="K8" s="107">
+        <v>1</v>
+      </c>
+      <c r="N8" s="107" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="117" t="s">
+      <c r="A9" s="107" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="117">
+      <c r="B9" s="107">
         <f>ROUND(ASINH(2),5)</f>
         <v>1.44364</v>
       </c>
-      <c r="C9" s="117">
+      <c r="C9" s="107">
         <v>1.44364</v>
       </c>
-      <c r="D9" s="117">
+      <c r="D9" s="107">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G9" s="117" t="s">
+      <c r="G9" s="107" t="s">
         <v>57</v>
       </c>
-      <c r="H9" s="117">
+      <c r="H9" s="107">
         <v>37</v>
       </c>
-      <c r="I9" s="117">
+      <c r="I9" s="107">
         <v>4890.1000000000004</v>
       </c>
-      <c r="J9" s="117">
+      <c r="J9" s="107">
         <v>5000</v>
       </c>
-      <c r="K9" s="117">
+      <c r="K9" s="107">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="117" t="s">
+      <c r="A10" s="107" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="117">
+      <c r="B10" s="107">
         <f>ROUND(ATAN(1),5)</f>
         <v>0.78539999999999999</v>
       </c>
-      <c r="C10" s="117">
+      <c r="C10" s="107">
         <v>0.78539999999999999</v>
       </c>
-      <c r="D10" s="117">
+      <c r="D10" s="107">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="117" t="s">
+      <c r="A11" s="107" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="117">
+      <c r="B11" s="107">
         <f>ROUND(ATAN2(-1,0),5)</f>
         <v>3.1415899999999999</v>
       </c>
-      <c r="C11" s="117">
+      <c r="C11" s="107">
         <v>3.1415899999999999</v>
       </c>
-      <c r="D11" s="117">
+      <c r="D11" s="107">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G11" s="117" t="s">
+      <c r="G11" s="107" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="117" t="s">
+      <c r="A12" s="107" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="117">
+      <c r="B12" s="107">
         <f>ROUND(ATANH(0.7),5)</f>
         <v>0.86729999999999996</v>
       </c>
-      <c r="C12" s="117">
+      <c r="C12" s="107">
         <v>0.86729999999999996</v>
       </c>
-      <c r="D12" s="117">
+      <c r="D12" s="107">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -9699,457 +9663,457 @@
       </c>
     </row>
     <row r="13" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="117" t="s">
+      <c r="A13" s="107" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="117">
+      <c r="B13" s="107">
         <f>ROUND(AVEDEV(I2:I9),5)</f>
         <v>2959.1624999999999</v>
       </c>
-      <c r="C13" s="117">
+      <c r="C13" s="107">
         <v>2959.1624999999999</v>
       </c>
-      <c r="D13" s="117">
+      <c r="D13" s="107">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G13" s="117" t="s">
+      <c r="G13" s="107" t="s">
         <v>46</v>
       </c>
-      <c r="H13" s="117" t="s">
+      <c r="H13" s="107" t="s">
         <v>63</v>
       </c>
-      <c r="I13" s="117" t="s">
+      <c r="I13" s="107" t="s">
         <v>64</v>
       </c>
-      <c r="J13" s="117" t="s">
+      <c r="J13" s="107" t="s">
         <v>65</v>
       </c>
-      <c r="K13" s="117" t="s">
+      <c r="K13" s="107" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="117" t="s">
+      <c r="A14" s="107" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="117">
+      <c r="B14" s="107">
         <f>ROUND(AVERAGE(H2:H9),5)</f>
         <v>26.25</v>
       </c>
-      <c r="C14" s="117">
+      <c r="C14" s="107">
         <v>26.25</v>
       </c>
-      <c r="D14" s="117">
+      <c r="D14" s="107">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="117" t="s">
+      <c r="A15" s="107" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="117">
+      <c r="B15" s="107">
         <f>AVERAGEA(G2:H9)</f>
         <v>13.125</v>
       </c>
-      <c r="C15" s="117">
+      <c r="C15" s="107">
         <v>13.125</v>
       </c>
-      <c r="D15" s="117">
+      <c r="D15" s="107">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="117" t="s">
+      <c r="A16" s="107" t="s">
         <v>69</v>
       </c>
-      <c r="B16" s="117">
+      <c r="B16" s="107">
         <f>ROUND(AVERAGEIF(J2:J9,"&gt;150000"),5)</f>
         <v>222797</v>
       </c>
-      <c r="C16" s="117">
+      <c r="C16" s="107">
         <v>222797</v>
       </c>
-      <c r="D16" s="117">
+      <c r="D16" s="107">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="117" t="s">
+      <c r="A17" s="107" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="117">
+      <c r="B17" s="107">
         <f>ROUND(AVERAGEIFS(I2:I9,H2:H9,"&gt;=30",K2:K9,"&lt;10"),5)</f>
         <v>8376.65</v>
       </c>
-      <c r="C17" s="117">
+      <c r="C17" s="107">
         <v>8376.65</v>
       </c>
-      <c r="D17" s="117">
+      <c r="D17" s="107">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="117" t="s">
+      <c r="A18" s="107" t="s">
         <v>71</v>
       </c>
-      <c r="B18" s="117">
+      <c r="B18" s="107">
         <f>CEILING(20.4,1)</f>
         <v>21</v>
       </c>
-      <c r="C18" s="117">
+      <c r="C18" s="107">
         <v>21</v>
       </c>
-      <c r="D18" s="117">
+      <c r="D18" s="107">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="117" t="s">
+      <c r="A19" s="107" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="117">
+      <c r="B19" s="107">
         <f>_xlfn.CEILING.MATH(-5.5,1,0)</f>
         <v>-5</v>
       </c>
-      <c r="C19" s="117">
+      <c r="C19" s="107">
         <v>-5</v>
       </c>
-      <c r="D19" s="117">
+      <c r="D19" s="107">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="117" t="s">
+      <c r="A20" s="107" t="s">
         <v>73</v>
       </c>
-      <c r="B20" s="117">
+      <c r="B20" s="107">
         <f>_xlfn.CEILING.PRECISE(230,100)</f>
         <v>300</v>
       </c>
-      <c r="C20" s="117">
+      <c r="C20" s="107">
         <v>300</v>
       </c>
-      <c r="D20" s="117">
+      <c r="D20" s="107">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="117" t="s">
+      <c r="A21" s="107" t="s">
         <v>74</v>
       </c>
-      <c r="B21" s="117" t="str">
+      <c r="B21" s="107" t="str">
         <f>CHAR(74)</f>
         <v>J</v>
       </c>
-      <c r="C21" s="117" t="s">
+      <c r="C21" s="107" t="s">
         <v>75</v>
       </c>
-      <c r="D21" s="117">
+      <c r="D21" s="107">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="117" t="s">
+      <c r="A22" s="107" t="s">
         <v>76</v>
       </c>
-      <c r="B22" s="117">
+      <c r="B22" s="107">
         <f>COLUMN(C4)</f>
         <v>3</v>
       </c>
-      <c r="C22" s="117">
+      <c r="C22" s="107">
         <v>3</v>
       </c>
-      <c r="D22" s="117">
+      <c r="D22" s="107">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="117" t="s">
+      <c r="A23" s="107" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="117">
+      <c r="B23" s="107">
         <f>COLUMNS(A5:D12)</f>
         <v>4</v>
       </c>
-      <c r="C23" s="117">
+      <c r="C23" s="107">
         <v>4</v>
       </c>
-      <c r="D23" s="117">
+      <c r="D23" s="107">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="117" t="s">
+      <c r="A24" s="107" t="s">
         <v>78</v>
       </c>
-      <c r="B24" s="117" t="str">
+      <c r="B24" s="107" t="str">
         <f>_xlfn.CONCAT(1,23)</f>
         <v>123</v>
       </c>
-      <c r="C24" s="117" t="str">
+      <c r="C24" s="107" t="str">
         <f>"123"</f>
         <v>123</v>
       </c>
-      <c r="D24" s="117">
+      <c r="D24" s="107">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="117" t="s">
+      <c r="A25" s="107" t="s">
         <v>79</v>
       </c>
-      <c r="B25" s="117" t="str">
+      <c r="B25" s="107" t="str">
         <f>CONCATENATE("BUT, ","MICHEL")</f>
         <v>BUT, MICHEL</v>
       </c>
-      <c r="C25" s="117" t="s">
+      <c r="C25" s="107" t="s">
         <v>80</v>
       </c>
-      <c r="D25" s="117">
+      <c r="D25" s="107">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="117" t="s">
+      <c r="A26" s="107" t="s">
         <v>81</v>
       </c>
-      <c r="B26" s="117">
+      <c r="B26" s="107">
         <f>ROUND(COS(PI()/3),2)</f>
         <v>0.5</v>
       </c>
-      <c r="C26" s="117">
+      <c r="C26" s="107">
         <v>0.5</v>
       </c>
-      <c r="D26" s="117">
+      <c r="D26" s="107">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="117" t="s">
+      <c r="A27" s="107" t="s">
         <v>82</v>
       </c>
-      <c r="B27" s="117">
+      <c r="B27" s="107">
         <f>ROUND(COSH(2),5)</f>
         <v>3.7622</v>
       </c>
-      <c r="C27" s="117">
+      <c r="C27" s="107">
         <v>3.7622</v>
       </c>
-      <c r="D27" s="117">
+      <c r="D27" s="107">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="117" t="s">
+      <c r="A28" s="107" t="s">
         <v>83</v>
       </c>
-      <c r="B28" s="117">
+      <c r="B28" s="107">
         <f>ROUND(_xlfn.COT(PI()/6),5)</f>
         <v>1.7320500000000001</v>
       </c>
-      <c r="C28" s="117">
+      <c r="C28" s="107">
         <f>ROUND(SQRT(3),5)</f>
         <v>1.7320500000000001</v>
       </c>
-      <c r="D28" s="117">
+      <c r="D28" s="107">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="117" t="s">
+      <c r="A29" s="107" t="s">
         <v>84</v>
       </c>
-      <c r="B29" s="117">
+      <c r="B29" s="107">
         <f>ROUND(_xlfn.COTH(0.5),5)</f>
         <v>2.1639499999999998</v>
       </c>
-      <c r="C29" s="117">
+      <c r="C29" s="107">
         <v>2.1639499999999998</v>
       </c>
-      <c r="D29" s="117">
+      <c r="D29" s="107">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="117" t="s">
+      <c r="A30" s="107" t="s">
         <v>85</v>
       </c>
-      <c r="B30" s="117">
+      <c r="B30" s="107">
         <f>COUNT(1,"a","5","2021-03-14")</f>
         <v>3</v>
       </c>
-      <c r="C30" s="117">
+      <c r="C30" s="107">
         <v>2</v>
       </c>
-      <c r="D30" s="117">
+      <c r="D30" s="107">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="117" t="s">
+      <c r="A31" s="107" t="s">
         <v>86</v>
       </c>
-      <c r="B31" s="117">
+      <c r="B31" s="107">
         <f>COUNTA(1,"a","5","2021-03-14")</f>
         <v>4</v>
       </c>
-      <c r="C31" s="117">
+      <c r="C31" s="107">
         <v>4</v>
       </c>
-      <c r="D31" s="117">
+      <c r="D31" s="107">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="117" t="s">
+      <c r="A32" s="107" t="s">
         <v>87</v>
       </c>
-      <c r="B32" s="117">
+      <c r="B32" s="107">
         <f>COUNTBLANK(F1:G1)</f>
         <v>1</v>
       </c>
-      <c r="C32" s="117">
-        <v>1</v>
-      </c>
-      <c r="D32" s="117">
+      <c r="C32" s="107">
+        <v>1</v>
+      </c>
+      <c r="D32" s="107">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="117" t="s">
+      <c r="A33" s="107" t="s">
         <v>88</v>
       </c>
-      <c r="B33" s="117">
+      <c r="B33" s="107">
         <f>COUNTIF(H2:H9,"&gt;30")</f>
         <v>2</v>
       </c>
-      <c r="C33" s="117">
+      <c r="C33" s="107">
         <v>2</v>
       </c>
-      <c r="D33" s="117">
+      <c r="D33" s="107">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="117" t="s">
+      <c r="A34" s="107" t="s">
         <v>89</v>
       </c>
-      <c r="B34" s="117">
+      <c r="B34" s="107">
         <f>COUNTIFS(H2:H9,"&gt;25",K2:K9,"&lt;4")</f>
         <v>3</v>
       </c>
-      <c r="C34" s="117">
+      <c r="C34" s="107">
         <v>3</v>
       </c>
-      <c r="D34" s="117">
+      <c r="D34" s="107">
         <f t="shared" ref="D34:D65" si="4">IF(B34=C34,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="117" t="s">
+      <c r="A35" s="107" t="s">
         <v>90</v>
       </c>
-      <c r="B35" s="117">
+      <c r="B35" s="107">
         <f>ROUND(COVAR(H2:H9,K2:K9),5)</f>
         <v>-2119.25</v>
       </c>
-      <c r="C35" s="117">
+      <c r="C35" s="107">
         <v>-2119.25</v>
       </c>
-      <c r="D35" s="117">
+      <c r="D35" s="107">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="117" t="s">
+      <c r="A36" s="107" t="s">
         <v>91</v>
       </c>
-      <c r="B36" s="117">
+      <c r="B36" s="107">
         <f>ROUND(_xlfn.COVARIANCE.P(K2:K9,H2:H9),5)</f>
         <v>-2119.25</v>
       </c>
-      <c r="C36" s="117">
+      <c r="C36" s="107">
         <v>-2119.25</v>
       </c>
-      <c r="D36" s="117">
+      <c r="D36" s="107">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="117" t="s">
+      <c r="A37" s="107" t="s">
         <v>92</v>
       </c>
-      <c r="B37" s="117">
+      <c r="B37" s="107">
         <f>ROUND(_xlfn.COVARIANCE.P(I2:I9,J2:J9),5)</f>
         <v>237217364.71641001</v>
       </c>
-      <c r="C37" s="117">
+      <c r="C37" s="107">
         <v>237217364.71641001</v>
       </c>
-      <c r="D37" s="117">
+      <c r="D37" s="107">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="117" t="s">
+      <c r="A38" s="107" t="s">
         <v>93</v>
       </c>
-      <c r="B38" s="117">
+      <c r="B38" s="107">
         <f>ROUND(_xlfn.CSC(PI()/4),5)</f>
         <v>1.41421</v>
       </c>
-      <c r="C38" s="117">
+      <c r="C38" s="107">
         <f>ROUND(SQRT(2),5)</f>
         <v>1.41421</v>
       </c>
-      <c r="D38" s="117">
+      <c r="D38" s="107">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="117" t="s">
+      <c r="A39" s="107" t="s">
         <v>94</v>
       </c>
-      <c r="B39" s="117">
+      <c r="B39" s="107">
         <f>ROUND(_xlfn.CSCH(PI()/3),5)</f>
         <v>0.80040999999999995</v>
       </c>
-      <c r="C39" s="117">
+      <c r="C39" s="107">
         <v>0.80040999999999995</v>
       </c>
-      <c r="D39" s="117">
+      <c r="D39" s="107">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="117" t="s">
+      <c r="A40" s="107" t="s">
         <v>95</v>
       </c>
       <c r="B40" s="18">
@@ -10159,287 +10123,287 @@
       <c r="C40" s="18">
         <v>43976</v>
       </c>
-      <c r="D40" s="117">
+      <c r="D40" s="107">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="117" t="s">
+      <c r="A41" s="107" t="s">
         <v>96</v>
       </c>
-      <c r="B41" s="117">
+      <c r="B41" s="107">
         <f>DATEVALUE("1969-08-15")</f>
         <v>25430</v>
       </c>
-      <c r="C41" s="117">
+      <c r="C41" s="107">
         <v>25430</v>
       </c>
-      <c r="D41" s="117">
+      <c r="D41" s="107">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="117" t="s">
+      <c r="A42" s="107" t="s">
         <v>97</v>
       </c>
-      <c r="B42" s="117">
+      <c r="B42" s="107">
         <f>ROUND(DAVERAGE(G1:K9,"Tot. Score",J12:J13),5)</f>
         <v>151434.625</v>
       </c>
-      <c r="C42" s="117">
+      <c r="C42" s="107">
         <v>151434.625</v>
       </c>
-      <c r="D42" s="117">
+      <c r="D42" s="107">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="117" t="s">
+      <c r="A43" s="107" t="s">
         <v>98</v>
       </c>
-      <c r="B43" s="117">
+      <c r="B43" s="107">
         <f>DAY("2020-03-17")</f>
         <v>17</v>
       </c>
-      <c r="C43" s="117">
+      <c r="C43" s="107">
         <v>17</v>
       </c>
-      <c r="D43" s="117">
+      <c r="D43" s="107">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="117" t="s">
+      <c r="A44" s="107" t="s">
         <v>99</v>
       </c>
-      <c r="B44" s="117">
+      <c r="B44" s="107">
         <f>_xlfn.DAYS("2022-03-17","2021-03-17")</f>
         <v>365</v>
       </c>
-      <c r="C44" s="117">
+      <c r="C44" s="107">
         <v>365</v>
       </c>
-      <c r="D44" s="117">
+      <c r="D44" s="107">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="117" t="s">
+      <c r="A45" s="107" t="s">
         <v>100</v>
       </c>
-      <c r="B45" s="117">
+      <c r="B45" s="107">
         <f>DCOUNT(G1:K9,"Name",H12:H13)</f>
         <v>0</v>
       </c>
-      <c r="C45" s="117">
+      <c r="C45" s="107">
         <v>0</v>
       </c>
-      <c r="D45" s="117">
+      <c r="D45" s="107">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="117" t="s">
+      <c r="A46" s="107" t="s">
         <v>101</v>
       </c>
-      <c r="B46" s="117">
+      <c r="B46" s="107">
         <f>DCOUNTA(G1:K9,"Name",H12:H13)</f>
         <v>3</v>
       </c>
-      <c r="C46" s="117">
+      <c r="C46" s="107">
         <v>3</v>
       </c>
-      <c r="D46" s="117">
+      <c r="D46" s="107">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="117" t="s">
+      <c r="A47" s="107" t="s">
         <v>102</v>
       </c>
-      <c r="B47" s="117">
+      <c r="B47" s="107">
         <f>_xlfn.DECIMAL(20,16)</f>
         <v>32</v>
       </c>
-      <c r="C47" s="117">
+      <c r="C47" s="107">
         <v>32</v>
       </c>
-      <c r="D47" s="117">
+      <c r="D47" s="107">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="117" t="s">
+      <c r="A48" s="107" t="s">
         <v>103</v>
       </c>
-      <c r="B48" s="117">
+      <c r="B48" s="107">
         <f>DEGREES(PI()/4)</f>
         <v>45</v>
       </c>
-      <c r="C48" s="117">
+      <c r="C48" s="107">
         <v>45</v>
       </c>
-      <c r="D48" s="117">
+      <c r="D48" s="107">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="117" t="s">
+      <c r="A49" s="107" t="s">
         <v>104</v>
       </c>
-      <c r="B49" s="117">
+      <c r="B49" s="107">
         <f>DGET(G1:K9,"Hours Played",G12:G13)</f>
         <v>252.4</v>
       </c>
-      <c r="C49" s="117">
+      <c r="C49" s="107">
         <v>252.4</v>
       </c>
-      <c r="D49" s="117">
+      <c r="D49" s="107">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="117" t="s">
+      <c r="A50" s="107" t="s">
         <v>105</v>
       </c>
-      <c r="B50" s="117">
+      <c r="B50" s="107">
         <f>DMAX(G1:K9,"Tot. Score",I12:I13)</f>
         <v>189576</v>
       </c>
-      <c r="C50" s="117">
+      <c r="C50" s="107">
         <f>J7</f>
         <v>189576</v>
       </c>
-      <c r="D50" s="117">
+      <c r="D50" s="107">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="117" t="s">
+      <c r="A51" s="107" t="s">
         <v>106</v>
       </c>
-      <c r="B51" s="117">
+      <c r="B51" s="107">
         <f>DMIN(G1:K9,"Tot. Score",H12:H13)</f>
         <v>5000</v>
       </c>
-      <c r="C51" s="117">
+      <c r="C51" s="107">
         <f>J9</f>
         <v>5000</v>
       </c>
-      <c r="D51" s="117">
+      <c r="D51" s="107">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="117" t="s">
+      <c r="A52" s="107" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="117">
+      <c r="B52" s="107">
         <f>DPRODUCT(G1:K9,"Age",K12:K13)</f>
         <v>333</v>
       </c>
-      <c r="C52" s="117">
+      <c r="C52" s="107">
         <v>333</v>
       </c>
-      <c r="D52" s="117">
+      <c r="D52" s="107">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="117" t="s">
+      <c r="A53" s="107" t="s">
         <v>108</v>
       </c>
-      <c r="B53" s="117">
+      <c r="B53" s="107">
         <f>ROUND(DSTDEV(G1:K9,"Age",H12:H13),5)</f>
         <v>6.0277099999999999</v>
       </c>
-      <c r="C53" s="117">
+      <c r="C53" s="107">
         <v>6.0277099999999999</v>
       </c>
-      <c r="D53" s="117">
+      <c r="D53" s="107">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="117" t="s">
+      <c r="A54" s="107" t="s">
         <v>109</v>
       </c>
-      <c r="B54" s="117">
+      <c r="B54" s="107">
         <f>ROUND(DSTDEVP(G1:K9,"Age",H12:H13),5)</f>
         <v>4.9216100000000003</v>
       </c>
-      <c r="C54" s="117">
+      <c r="C54" s="107">
         <v>4.9216100000000003</v>
       </c>
-      <c r="D54" s="117">
+      <c r="D54" s="107">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="117" t="s">
+      <c r="A55" s="107" t="s">
         <v>110</v>
       </c>
-      <c r="B55" s="117">
+      <c r="B55" s="107">
         <f>DSUM(G1:K9,"Age",I12:I13)</f>
         <v>101</v>
       </c>
-      <c r="C55" s="117">
+      <c r="C55" s="107">
         <v>101</v>
       </c>
-      <c r="D55" s="117">
+      <c r="D55" s="107">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="117" t="s">
+      <c r="A56" s="107" t="s">
         <v>111</v>
       </c>
-      <c r="B56" s="117">
+      <c r="B56" s="107">
         <f>ROUND(DVAR(G1:K9,"Hours Played",H12:H13),5)</f>
         <v>17560207.923330002</v>
       </c>
-      <c r="C56" s="117">
+      <c r="C56" s="107">
         <v>17560207.923330002</v>
       </c>
-      <c r="D56" s="117">
+      <c r="D56" s="107">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="117" t="s">
+      <c r="A57" s="107" t="s">
         <v>112</v>
       </c>
-      <c r="B57" s="117">
+      <c r="B57" s="107">
         <f>ROUND(DVARP(G1:K9,"Hours Played",H12:H13),5)</f>
         <v>11706805.28222</v>
       </c>
-      <c r="C57" s="117">
+      <c r="C57" s="107">
         <v>11706805.28222</v>
       </c>
-      <c r="D57" s="117">
+      <c r="D57" s="107">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="117" t="s">
+      <c r="A58" s="107" t="s">
         <v>113</v>
       </c>
       <c r="B58" s="18">
@@ -10449,13 +10413,13 @@
       <c r="C58" s="18">
         <v>25345</v>
       </c>
-      <c r="D58" s="117">
+      <c r="D58" s="107">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="117" t="s">
+      <c r="A59" s="107" t="s">
         <v>114</v>
       </c>
       <c r="B59" s="18">
@@ -10465,1311 +10429,1311 @@
       <c r="C59" s="18">
         <v>44074</v>
       </c>
-      <c r="D59" s="117">
+      <c r="D59" s="107">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="117" t="s">
+      <c r="A60" s="107" t="s">
         <v>115</v>
       </c>
-      <c r="B60" s="117" t="b">
+      <c r="B60" s="107" t="b">
         <f>EXACT("AbsSdf%","AbsSdf%")</f>
         <v>1</v>
       </c>
-      <c r="C60" s="117" t="b">
-        <v>1</v>
-      </c>
-      <c r="D60" s="117">
+      <c r="C60" s="107" t="b">
+        <v>1</v>
+      </c>
+      <c r="D60" s="107">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="117" t="s">
+      <c r="A61" s="107" t="s">
         <v>116</v>
       </c>
-      <c r="B61" s="117">
+      <c r="B61" s="107">
         <f>ROUND(EXP(4),5)</f>
         <v>54.598149999999997</v>
       </c>
-      <c r="C61" s="117">
+      <c r="C61" s="107">
         <v>54.598149999999997</v>
       </c>
-      <c r="D61" s="117">
+      <c r="D61" s="107">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="117" t="s">
+      <c r="A62" s="107" t="s">
         <v>117</v>
       </c>
-      <c r="B62" s="117">
+      <c r="B62" s="107">
         <f>FIND("A","qbdahbaazo A")</f>
         <v>12</v>
       </c>
-      <c r="C62" s="117">
+      <c r="C62" s="107">
         <v>12</v>
       </c>
-      <c r="D62" s="117">
+      <c r="D62" s="107">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="117" t="s">
+      <c r="A63" s="107" t="s">
         <v>118</v>
       </c>
-      <c r="B63" s="117">
+      <c r="B63" s="107">
         <f>FLOOR(5.5,2)</f>
         <v>4</v>
       </c>
-      <c r="C63" s="117">
+      <c r="C63" s="107">
         <v>4</v>
       </c>
-      <c r="D63" s="117">
+      <c r="D63" s="107">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="117" t="s">
+      <c r="A64" s="107" t="s">
         <v>119</v>
       </c>
-      <c r="B64" s="117">
+      <c r="B64" s="107">
         <f>_xlfn.FLOOR.MATH(-5.55,2,1)</f>
         <v>-4</v>
       </c>
-      <c r="C64" s="117">
+      <c r="C64" s="107">
         <v>-4</v>
       </c>
-      <c r="D64" s="117">
+      <c r="D64" s="107">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="117" t="s">
+      <c r="A65" s="107" t="s">
         <v>120</v>
       </c>
-      <c r="B65" s="117">
+      <c r="B65" s="107">
         <f>_xlfn.FLOOR.PRECISE(199,100)</f>
         <v>100</v>
       </c>
-      <c r="C65" s="117">
+      <c r="C65" s="107">
         <v>100</v>
       </c>
-      <c r="D65" s="117">
+      <c r="D65" s="107">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="117" t="s">
+      <c r="A66" s="107" t="s">
         <v>121</v>
       </c>
-      <c r="B66" s="117">
+      <c r="B66" s="107">
         <f>HLOOKUP("Tot. Score",H1:K9,4,FALSE)</f>
         <v>110120.5</v>
       </c>
-      <c r="C66" s="117">
+      <c r="C66" s="107">
         <v>110120.5</v>
       </c>
-      <c r="D66" s="117">
+      <c r="D66" s="107">
         <f t="shared" ref="D66:D97" si="5">IF(B66=C66,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="117" t="s">
+      <c r="A67" s="107" t="s">
         <v>122</v>
       </c>
-      <c r="B67" s="117">
+      <c r="B67" s="107">
         <f>HOUR("02:14:56")</f>
         <v>2</v>
       </c>
-      <c r="C67" s="117">
+      <c r="C67" s="107">
         <v>2</v>
       </c>
-      <c r="D67" s="117">
+      <c r="D67" s="107">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="117" t="s">
+      <c r="A68" s="107" t="s">
         <v>123</v>
       </c>
-      <c r="B68" s="117" t="str">
+      <c r="B68" s="107" t="str">
         <f>IF(TRUE,"TABOURET","JAMBON")</f>
         <v>TABOURET</v>
       </c>
-      <c r="C68" s="117" t="s">
+      <c r="C68" s="107" t="s">
         <v>124</v>
       </c>
-      <c r="D68" s="117">
+      <c r="D68" s="107">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="117" t="s">
+      <c r="A69" s="107" t="s">
         <v>125</v>
       </c>
-      <c r="B69" s="117" t="str">
+      <c r="B69" s="107" t="str">
         <f>IFERROR(0/0,"no diving by zero.")</f>
         <v>no diving by zero.</v>
       </c>
-      <c r="C69" s="117" t="s">
+      <c r="C69" s="107" t="s">
         <v>126</v>
       </c>
-      <c r="D69" s="117">
+      <c r="D69" s="107">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="117" t="s">
+      <c r="A70" s="107" t="s">
         <v>127</v>
       </c>
-      <c r="B70" s="117" t="str">
+      <c r="B70" s="107" t="str">
         <f>_xlfn.IFS($H2&gt;$H3,"first player is older",$H3&gt;$H2,"second player is older")</f>
         <v>first player is older</v>
       </c>
-      <c r="C70" s="117" t="s">
+      <c r="C70" s="107" t="s">
         <v>128</v>
       </c>
-      <c r="D70" s="117">
+      <c r="D70" s="107">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="117" t="s">
+      <c r="A71" s="107" t="s">
         <v>129</v>
       </c>
-      <c r="B71" s="117" t="b">
+      <c r="B71" s="107" t="b">
         <f>ISERROR(0/0)</f>
         <v>1</v>
       </c>
-      <c r="C71" s="117" t="b">
-        <v>1</v>
-      </c>
-      <c r="D71" s="117">
+      <c r="C71" s="107" t="b">
+        <v>1</v>
+      </c>
+      <c r="D71" s="107">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="117" t="s">
+      <c r="A72" s="107" t="s">
         <v>130</v>
       </c>
-      <c r="B72" s="117" t="b">
+      <c r="B72" s="107" t="b">
         <f>ISEVEN(3)</f>
         <v>0</v>
       </c>
-      <c r="C72" s="117" t="b">
+      <c r="C72" s="107" t="b">
         <v>0</v>
       </c>
-      <c r="D72" s="117">
+      <c r="D72" s="107">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="117" t="s">
+      <c r="A73" s="107" t="s">
         <v>131</v>
       </c>
-      <c r="B73" s="117" t="b">
+      <c r="B73" s="107" t="b">
         <f>ISLOGICAL("TRUE")</f>
         <v>0</v>
       </c>
-      <c r="C73" s="117" t="b">
+      <c r="C73" s="107" t="b">
         <v>0</v>
       </c>
-      <c r="D73" s="117">
+      <c r="D73" s="107">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="117" t="s">
+      <c r="A74" s="107" t="s">
         <v>132</v>
       </c>
-      <c r="B74" s="117" t="b">
+      <c r="B74" s="107" t="b">
         <f>ISNONTEXT(TRUE)</f>
         <v>1</v>
       </c>
-      <c r="C74" s="117" t="b">
-        <v>1</v>
-      </c>
-      <c r="D74" s="117">
+      <c r="C74" s="107" t="b">
+        <v>1</v>
+      </c>
+      <c r="D74" s="107">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="117" t="s">
+      <c r="A75" s="107" t="s">
         <v>133</v>
       </c>
-      <c r="B75" s="117" t="b">
+      <c r="B75" s="107" t="b">
         <f>ISNUMBER(1231.5)</f>
         <v>1</v>
       </c>
-      <c r="C75" s="117" t="b">
-        <v>1</v>
-      </c>
-      <c r="D75" s="117">
+      <c r="C75" s="107" t="b">
+        <v>1</v>
+      </c>
+      <c r="D75" s="107">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="117" t="s">
+      <c r="A76" s="107" t="s">
         <v>134</v>
       </c>
-      <c r="B76" s="117">
+      <c r="B76" s="107">
         <f>ISO.CEILING(-7.89)</f>
         <v>-7</v>
       </c>
-      <c r="C76" s="117">
+      <c r="C76" s="107">
         <v>-7</v>
       </c>
-      <c r="D76" s="117">
+      <c r="D76" s="107">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="117" t="s">
+      <c r="A77" s="107" t="s">
         <v>135</v>
       </c>
-      <c r="B77" s="117" t="b">
+      <c r="B77" s="107" t="b">
         <f>ISODD(4)</f>
         <v>0</v>
       </c>
-      <c r="C77" s="117" t="b">
+      <c r="C77" s="107" t="b">
         <v>0</v>
       </c>
-      <c r="D77" s="117">
+      <c r="D77" s="107">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="117" t="s">
+      <c r="A78" s="107" t="s">
         <v>136</v>
       </c>
-      <c r="B78" s="117">
+      <c r="B78" s="107">
         <f>_xlfn.ISOWEEKNUM("2016-01-03")</f>
         <v>53</v>
       </c>
-      <c r="C78" s="117">
+      <c r="C78" s="107">
         <v>53</v>
       </c>
-      <c r="D78" s="117">
+      <c r="D78" s="107">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="117" t="s">
+      <c r="A79" s="107" t="s">
         <v>137</v>
       </c>
-      <c r="B79" s="117" t="b">
+      <c r="B79" s="107" t="b">
         <f>ISTEXT("123")</f>
         <v>1</v>
       </c>
-      <c r="C79" s="117" t="b">
-        <v>1</v>
-      </c>
-      <c r="D79" s="117">
+      <c r="C79" s="107" t="b">
+        <v>1</v>
+      </c>
+      <c r="D79" s="107">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="117" t="s">
+      <c r="A80" s="107" t="s">
         <v>138</v>
       </c>
-      <c r="B80" s="117">
+      <c r="B80" s="107">
         <f>LARGE(H2:H9,3)</f>
         <v>30</v>
       </c>
-      <c r="C80" s="117">
+      <c r="C80" s="107">
         <v>30</v>
       </c>
-      <c r="D80" s="117">
+      <c r="D80" s="107">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="117" t="s">
+      <c r="A81" s="107" t="s">
         <v>139</v>
       </c>
-      <c r="B81" s="117" t="str">
+      <c r="B81" s="107" t="str">
         <f>LEFT("Mich",4)</f>
         <v>Mich</v>
       </c>
-      <c r="C81" s="117" t="s">
+      <c r="C81" s="107" t="s">
         <v>140</v>
       </c>
-      <c r="D81" s="117">
+      <c r="D81" s="107">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="117" t="s">
+      <c r="A82" s="107" t="s">
         <v>141</v>
       </c>
-      <c r="B82" s="117">
+      <c r="B82" s="107">
         <f>LEN("anticonstitutionnellement")</f>
         <v>25</v>
       </c>
-      <c r="C82" s="117">
+      <c r="C82" s="107">
         <v>25</v>
       </c>
-      <c r="D82" s="117">
+      <c r="D82" s="107">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="117" t="s">
+      <c r="A83" s="107" t="s">
         <v>142</v>
       </c>
-      <c r="B83" s="117">
+      <c r="B83" s="107">
         <f>ROUND(LN(2),5)</f>
         <v>0.69315000000000004</v>
       </c>
-      <c r="C83" s="117">
+      <c r="C83" s="107">
         <v>0.69315000000000004</v>
       </c>
-      <c r="D83" s="117">
+      <c r="D83" s="107">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="117" t="s">
+      <c r="A84" s="107" t="s">
         <v>143</v>
       </c>
-      <c r="B84" s="117">
+      <c r="B84" s="107">
         <f>LOOKUP(23000,H3:J3,H5:J5)</f>
         <v>50024</v>
       </c>
-      <c r="C84" s="117">
+      <c r="C84" s="107">
         <v>50024</v>
       </c>
-      <c r="D84" s="117">
+      <c r="D84" s="107">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="117" t="s">
+      <c r="A85" s="107" t="s">
         <v>144</v>
       </c>
-      <c r="B85" s="117" t="str">
+      <c r="B85" s="107" t="str">
         <f>LOWER("オAドB")</f>
         <v>オaドb</v>
       </c>
-      <c r="C85" s="117" t="s">
+      <c r="C85" s="107" t="s">
         <v>145</v>
       </c>
-      <c r="D85" s="117">
+      <c r="D85" s="107">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="117" t="s">
+      <c r="A86" s="107" t="s">
         <v>146</v>
       </c>
-      <c r="B86" s="117">
+      <c r="B86" s="107">
         <f>MATCH(42,H2:H9,0)</f>
         <v>4</v>
       </c>
-      <c r="C86" s="117">
+      <c r="C86" s="107">
         <v>4</v>
       </c>
-      <c r="D86" s="117">
+      <c r="D86" s="107">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="117" t="s">
+      <c r="A87" s="107" t="s">
         <v>147</v>
       </c>
-      <c r="B87" s="117">
+      <c r="B87" s="107">
         <f>MAX(N1:N8)</f>
         <v>0.6</v>
       </c>
-      <c r="C87" s="117">
+      <c r="C87" s="107">
         <v>0.6</v>
       </c>
-      <c r="D87" s="117">
+      <c r="D87" s="107">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="117" t="s">
+      <c r="A88" s="107" t="s">
         <v>148</v>
       </c>
-      <c r="B88" s="117">
+      <c r="B88" s="107">
         <f>MAXA(N1:N8)</f>
         <v>1</v>
       </c>
-      <c r="C88" s="117">
-        <v>1</v>
-      </c>
-      <c r="D88" s="117">
+      <c r="C88" s="107">
+        <v>1</v>
+      </c>
+      <c r="D88" s="107">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="117" t="s">
+      <c r="A89" s="107" t="s">
         <v>149</v>
       </c>
-      <c r="B89" s="117">
+      <c r="B89" s="107">
         <f>_xlfn.MAXIFS(H2:H9,K2:K9,"&lt;20",K2:K9,"&lt;&gt;4")</f>
         <v>30</v>
       </c>
-      <c r="C89" s="117">
+      <c r="C89" s="107">
         <v>30</v>
       </c>
-      <c r="D89" s="117">
+      <c r="D89" s="107">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="117" t="s">
+      <c r="A90" s="107" t="s">
         <v>150</v>
       </c>
-      <c r="B90" s="117">
+      <c r="B90" s="107">
         <f>MEDIAN(-1,6,7,234,163845)</f>
         <v>7</v>
       </c>
-      <c r="C90" s="117">
+      <c r="C90" s="107">
         <v>7</v>
       </c>
-      <c r="D90" s="117">
+      <c r="D90" s="107">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="117" t="s">
+      <c r="A91" s="107" t="s">
         <v>151</v>
       </c>
-      <c r="B91" s="117">
+      <c r="B91" s="107">
         <f>MIN(N1:N8)</f>
         <v>0.1</v>
       </c>
-      <c r="C91" s="117">
+      <c r="C91" s="107">
         <v>0.1</v>
       </c>
-      <c r="D91" s="117">
+      <c r="D91" s="107">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="117" t="s">
+      <c r="A92" s="107" t="s">
         <v>152</v>
       </c>
-      <c r="B92" s="117">
+      <c r="B92" s="107">
         <f>MINA(N1:N8)</f>
         <v>0</v>
       </c>
-      <c r="C92" s="117">
+      <c r="C92" s="107">
         <v>0</v>
       </c>
-      <c r="D92" s="117">
+      <c r="D92" s="107">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="117" t="s">
+      <c r="A93" s="107" t="s">
         <v>153</v>
       </c>
-      <c r="B93" s="117">
+      <c r="B93" s="107">
         <f>_xlfn.MINIFS(J2:J9,H2:H9,"&gt;20")</f>
         <v>5000</v>
       </c>
-      <c r="C93" s="117">
+      <c r="C93" s="107">
         <v>5000</v>
       </c>
-      <c r="D93" s="117">
+      <c r="D93" s="107">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="117" t="s">
+      <c r="A94" s="107" t="s">
         <v>154</v>
       </c>
-      <c r="B94" s="117">
+      <c r="B94" s="107">
         <f>MINUTE(0.126)</f>
         <v>1</v>
       </c>
-      <c r="C94" s="117">
-        <v>1</v>
-      </c>
-      <c r="D94" s="117">
+      <c r="C94" s="107">
+        <v>1</v>
+      </c>
+      <c r="D94" s="107">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="117" t="s">
+      <c r="A95" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="B95" s="117">
+      <c r="B95" s="107">
         <f>MOD(42,12)</f>
         <v>6</v>
       </c>
-      <c r="C95" s="117">
+      <c r="C95" s="107">
         <v>6</v>
       </c>
-      <c r="D95" s="117">
+      <c r="D95" s="107">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="117" t="s">
+      <c r="A96" s="107" t="s">
         <v>156</v>
       </c>
-      <c r="B96" s="117">
+      <c r="B96" s="107">
         <f>MONTH("1954-05-02")</f>
         <v>5</v>
       </c>
-      <c r="C96" s="117">
+      <c r="C96" s="107">
         <v>5</v>
       </c>
-      <c r="D96" s="117">
+      <c r="D96" s="107">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="117" t="s">
+      <c r="A97" s="107" t="s">
         <v>157</v>
       </c>
-      <c r="B97" s="117">
+      <c r="B97" s="107">
         <f>NETWORKDAYS("2013-01-01","2013-02-01")</f>
         <v>24</v>
       </c>
-      <c r="C97" s="117">
+      <c r="C97" s="107">
         <v>24</v>
       </c>
-      <c r="D97" s="117">
+      <c r="D97" s="107">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="117" t="s">
+      <c r="A98" s="107" t="s">
         <v>158</v>
       </c>
-      <c r="B98" s="117">
+      <c r="B98" s="107">
         <f>NETWORKDAYS.INTL("2013-01-01","2013-02-01","0000111")</f>
         <v>19</v>
       </c>
-      <c r="C98" s="117">
+      <c r="C98" s="107">
         <v>19</v>
       </c>
-      <c r="D98" s="117">
+      <c r="D98" s="107">
         <f t="shared" ref="D98:D99" si="6">IF(B98=C98,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="117" t="s">
+      <c r="A99" s="107" t="s">
         <v>159</v>
       </c>
-      <c r="B99" s="117" t="b">
+      <c r="B99" s="107" t="b">
         <f>NOT(FALSE)</f>
         <v>1</v>
       </c>
-      <c r="C99" s="117" t="b">
-        <v>1</v>
-      </c>
-      <c r="D99" s="117">
+      <c r="C99" s="107" t="b">
+        <v>1</v>
+      </c>
+      <c r="D99" s="107">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="117" t="s">
+      <c r="A100" s="107" t="s">
         <v>160</v>
       </c>
       <c r="B100" s="19">
         <f ca="1">NOW()</f>
-        <v>45903.380486458336</v>
-      </c>
-      <c r="D100" s="117">
+        <v>45903.620136342593</v>
+      </c>
+      <c r="D100" s="107">
         <f ca="1">IF(ISNUMBER(B100),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="117" t="s">
+      <c r="A101" s="107" t="s">
         <v>161</v>
       </c>
-      <c r="B101" s="117">
+      <c r="B101" s="107">
         <f>ODD(4)</f>
         <v>5</v>
       </c>
-      <c r="C101" s="117">
+      <c r="C101" s="107">
         <v>5</v>
       </c>
-      <c r="D101" s="117">
+      <c r="D101" s="107">
         <f t="shared" ref="D101:D111" si="7">IF(B101=C101,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="117" t="s">
+      <c r="A102" s="107" t="s">
         <v>162</v>
       </c>
-      <c r="B102" s="117" t="b">
+      <c r="B102" s="107" t="b">
         <f>OR("true",FALSE)</f>
         <v>1</v>
       </c>
-      <c r="C102" s="117" t="b">
-        <v>1</v>
-      </c>
-      <c r="D102" s="117">
+      <c r="C102" s="107" t="b">
+        <v>1</v>
+      </c>
+      <c r="D102" s="107">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="117" t="s">
+      <c r="A103" s="107" t="s">
         <v>163</v>
       </c>
-      <c r="B103" s="117">
+      <c r="B103" s="107">
         <f>PERCENTILE(N1:N5,1)</f>
         <v>0.6</v>
       </c>
-      <c r="C103" s="117">
+      <c r="C103" s="107">
         <v>0.6</v>
       </c>
-      <c r="D103" s="117">
+      <c r="D103" s="107">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="117" t="s">
+      <c r="A104" s="107" t="s">
         <v>164</v>
       </c>
-      <c r="B104" s="117">
+      <c r="B104" s="107">
         <f>_xlfn.PERCENTILE.EXC(N1:N5,0.5)</f>
         <v>0.4</v>
       </c>
-      <c r="C104" s="117">
+      <c r="C104" s="107">
         <v>0.4</v>
       </c>
-      <c r="D104" s="117">
+      <c r="D104" s="107">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="117" t="s">
+      <c r="A105" s="107" t="s">
         <v>165</v>
       </c>
-      <c r="B105" s="117">
+      <c r="B105" s="107">
         <f>_xlfn.PERCENTILE.INC(N1:N5,0)</f>
         <v>0.1</v>
       </c>
-      <c r="C105" s="117">
+      <c r="C105" s="107">
         <v>0.1</v>
       </c>
-      <c r="D105" s="117">
+      <c r="D105" s="107">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="117" t="s">
+      <c r="A106" s="107" t="s">
         <v>166</v>
       </c>
-      <c r="B106" s="117">
+      <c r="B106" s="107">
         <f>ROUND(PI(),5)</f>
         <v>3.1415899999999999</v>
       </c>
-      <c r="C106" s="117">
+      <c r="C106" s="107">
         <v>3.1415899999999999</v>
       </c>
-      <c r="D106" s="117">
+      <c r="D106" s="107">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="117" t="s">
+      <c r="A107" s="107" t="s">
         <v>167</v>
       </c>
-      <c r="B107" s="117">
+      <c r="B107" s="107">
         <f>POWER(42,2)</f>
         <v>1764</v>
       </c>
-      <c r="C107" s="117">
+      <c r="C107" s="107">
         <v>1764</v>
       </c>
-      <c r="D107" s="117">
+      <c r="D107" s="107">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="117" t="s">
+      <c r="A108" s="107" t="s">
         <v>168</v>
       </c>
-      <c r="B108" s="117">
+      <c r="B108" s="107">
         <f>PRODUCT(1,2,3)</f>
         <v>6</v>
       </c>
-      <c r="C108" s="117">
+      <c r="C108" s="107">
         <v>6</v>
       </c>
-      <c r="D108" s="117">
+      <c r="D108" s="107">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="117" t="s">
+      <c r="A109" s="107" t="s">
         <v>169</v>
       </c>
-      <c r="B109" s="117">
+      <c r="B109" s="107">
         <f>QUARTILE(N1:N5,0)</f>
         <v>0.1</v>
       </c>
-      <c r="C109" s="117">
+      <c r="C109" s="107">
         <v>0.1</v>
       </c>
-      <c r="D109" s="117">
+      <c r="D109" s="107">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="117" t="s">
+      <c r="A110" s="107" t="s">
         <v>170</v>
       </c>
-      <c r="B110" s="117">
+      <c r="B110" s="107">
         <f>ROUND(_xlfn.QUARTILE.EXC(N1:N5,1),5)</f>
         <v>0.15</v>
       </c>
-      <c r="C110" s="117">
+      <c r="C110" s="107">
         <v>0.15</v>
       </c>
-      <c r="D110" s="117">
+      <c r="D110" s="107">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="117" t="s">
+      <c r="A111" s="107" t="s">
         <v>171</v>
       </c>
-      <c r="B111" s="117">
+      <c r="B111" s="107">
         <f>_xlfn.QUARTILE.INC(N1:N5,4)</f>
         <v>0.6</v>
       </c>
-      <c r="C111" s="117">
+      <c r="C111" s="107">
         <v>0.6</v>
       </c>
-      <c r="D111" s="117">
+      <c r="D111" s="107">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="117"/>
-      <c r="B112" s="117"/>
-      <c r="D112" s="117"/>
+      <c r="A112" s="107"/>
+      <c r="B112" s="107"/>
+      <c r="D112" s="107"/>
     </row>
     <row r="113" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="117" t="s">
+      <c r="A113" s="107" t="s">
         <v>172</v>
       </c>
-      <c r="B113" s="117">
+      <c r="B113" s="107">
         <f ca="1">RANDBETWEEN(1.1,2)</f>
         <v>2</v>
       </c>
-      <c r="C113" s="117">
+      <c r="C113" s="107">
         <v>2</v>
       </c>
-      <c r="D113" s="117">
+      <c r="D113" s="107">
         <f t="shared" ref="D113:D143" ca="1" si="8">IF(B113=C113,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="117" t="s">
+      <c r="A114" s="107" t="s">
         <v>173</v>
       </c>
-      <c r="B114" s="117" t="str">
+      <c r="B114" s="107" t="str">
         <f>REPLACE("ABZ",2,1,"Y")</f>
         <v>AYZ</v>
       </c>
-      <c r="C114" s="117" t="s">
+      <c r="C114" s="107" t="s">
         <v>174</v>
       </c>
-      <c r="D114" s="117">
+      <c r="D114" s="107">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="117" t="s">
+      <c r="A115" s="107" t="s">
         <v>175</v>
       </c>
-      <c r="B115" s="117" t="str">
+      <c r="B115" s="107" t="str">
         <f>RIGHT("kikou",2)</f>
         <v>ou</v>
       </c>
-      <c r="C115" s="117" t="s">
+      <c r="C115" s="107" t="s">
         <v>176</v>
       </c>
-      <c r="D115" s="117">
+      <c r="D115" s="107">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="117" t="s">
+      <c r="A116" s="107" t="s">
         <v>177</v>
       </c>
-      <c r="B116" s="117">
+      <c r="B116" s="107">
         <f>ROUND(49.9,0)</f>
         <v>50</v>
       </c>
-      <c r="C116" s="117">
+      <c r="C116" s="107">
         <v>50</v>
       </c>
-      <c r="D116" s="117">
+      <c r="D116" s="107">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="117" t="s">
+      <c r="A117" s="107" t="s">
         <v>178</v>
       </c>
-      <c r="B117" s="117">
+      <c r="B117" s="107">
         <f>ROUNDDOWN(42,-1)</f>
         <v>40</v>
       </c>
-      <c r="C117" s="117">
+      <c r="C117" s="107">
         <v>40</v>
       </c>
-      <c r="D117" s="117">
+      <c r="D117" s="107">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="117" t="s">
+      <c r="A118" s="107" t="s">
         <v>179</v>
       </c>
-      <c r="B118" s="117">
+      <c r="B118" s="107">
         <f>ROUNDUP(-1.6,0)</f>
         <v>-2</v>
       </c>
-      <c r="C118" s="117">
+      <c r="C118" s="107">
         <v>-2</v>
       </c>
-      <c r="D118" s="117">
+      <c r="D118" s="107">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="117" t="s">
+      <c r="A119" s="107" t="s">
         <v>180</v>
       </c>
-      <c r="B119" s="117">
+      <c r="B119" s="107">
         <f>ROW(A234)</f>
         <v>234</v>
       </c>
-      <c r="C119" s="117">
+      <c r="C119" s="107">
         <v>234</v>
       </c>
-      <c r="D119" s="117">
+      <c r="D119" s="107">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="117" t="s">
+      <c r="A120" s="107" t="s">
         <v>181</v>
       </c>
-      <c r="B120" s="117">
+      <c r="B120" s="107">
         <f>ROWS(B3:C40)</f>
         <v>38</v>
       </c>
-      <c r="C120" s="117">
+      <c r="C120" s="107">
         <v>38</v>
       </c>
-      <c r="D120" s="117">
+      <c r="D120" s="107">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="117" t="s">
+      <c r="A121" s="107" t="s">
         <v>182</v>
       </c>
-      <c r="B121" s="117">
+      <c r="B121" s="107">
         <f>SEARCH("C","ABCD")</f>
         <v>3</v>
       </c>
-      <c r="C121" s="117">
+      <c r="C121" s="107">
         <v>3</v>
       </c>
-      <c r="D121" s="117">
+      <c r="D121" s="107">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="117" t="s">
+      <c r="A122" s="107" t="s">
         <v>183</v>
       </c>
-      <c r="B122" s="117">
+      <c r="B122" s="107">
         <f>ROUND(_xlfn.SEC(PI()/3),5)</f>
         <v>2</v>
       </c>
-      <c r="C122" s="117">
+      <c r="C122" s="107">
         <v>2</v>
       </c>
-      <c r="D122" s="117">
+      <c r="D122" s="107">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="117" t="s">
+      <c r="A123" s="107" t="s">
         <v>184</v>
       </c>
-      <c r="B123" s="117">
+      <c r="B123" s="107">
         <f>ROUND(_xlfn.SECH(1),5)</f>
         <v>0.64805000000000001</v>
       </c>
-      <c r="C123" s="117">
+      <c r="C123" s="107">
         <v>0.64805000000000001</v>
       </c>
-      <c r="D123" s="117">
+      <c r="D123" s="107">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="117" t="s">
+      <c r="A124" s="107" t="s">
         <v>185</v>
       </c>
-      <c r="B124" s="117">
+      <c r="B124" s="107">
         <f>SECOND("00:21:42")</f>
         <v>42</v>
       </c>
-      <c r="C124" s="117">
+      <c r="C124" s="107">
         <v>42</v>
       </c>
-      <c r="D124" s="117">
+      <c r="D124" s="107">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="117" t="s">
+      <c r="A125" s="107" t="s">
         <v>186</v>
       </c>
-      <c r="B125" s="117">
+      <c r="B125" s="107">
         <f>ROUND(SIN(PI()/6),5)</f>
         <v>0.5</v>
       </c>
-      <c r="C125" s="117">
+      <c r="C125" s="107">
         <v>0.5</v>
       </c>
-      <c r="D125" s="117">
+      <c r="D125" s="107">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="117" t="s">
+      <c r="A126" s="107" t="s">
         <v>187</v>
       </c>
-      <c r="B126" s="117">
+      <c r="B126" s="107">
         <f>ROUND(SINH(1),5)</f>
         <v>1.1752</v>
       </c>
-      <c r="C126" s="117">
+      <c r="C126" s="107">
         <v>1.1752</v>
       </c>
-      <c r="D126" s="117">
+      <c r="D126" s="107">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="117" t="s">
+      <c r="A127" s="107" t="s">
         <v>188</v>
       </c>
-      <c r="B127" s="117">
+      <c r="B127" s="107">
         <f>SMALL(H2:H9,3)</f>
         <v>26</v>
       </c>
-      <c r="C127" s="117">
+      <c r="C127" s="107">
         <v>26</v>
       </c>
-      <c r="D127" s="117">
+      <c r="D127" s="107">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="117" t="s">
+      <c r="A128" s="107" t="s">
         <v>189</v>
       </c>
-      <c r="B128" s="117">
+      <c r="B128" s="107">
         <f>SQRT(4)</f>
         <v>2</v>
       </c>
-      <c r="C128" s="117">
+      <c r="C128" s="107">
         <v>2</v>
       </c>
-      <c r="D128" s="117">
+      <c r="D128" s="107">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="117" t="s">
+      <c r="A129" s="107" t="s">
         <v>190</v>
       </c>
-      <c r="B129" s="117">
+      <c r="B129" s="107">
         <f>STDEV(-2,0,2)</f>
         <v>2</v>
       </c>
-      <c r="C129" s="117">
+      <c r="C129" s="107">
         <v>2</v>
       </c>
-      <c r="D129" s="117">
+      <c r="D129" s="107">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="117" t="s">
+      <c r="A130" s="107" t="s">
         <v>191</v>
       </c>
-      <c r="B130" s="117">
+      <c r="B130" s="107">
         <f>_xlfn.STDEV.P(2,4)</f>
         <v>1</v>
       </c>
-      <c r="C130" s="117">
-        <v>1</v>
-      </c>
-      <c r="D130" s="117">
+      <c r="C130" s="107">
+        <v>1</v>
+      </c>
+      <c r="D130" s="107">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="117" t="s">
+      <c r="A131" s="107" t="s">
         <v>192</v>
       </c>
-      <c r="B131" s="117">
+      <c r="B131" s="107">
         <f>_xlfn.STDEV.S(2,4,6)</f>
         <v>2</v>
       </c>
-      <c r="C131" s="117">
+      <c r="C131" s="107">
         <v>2</v>
       </c>
-      <c r="D131" s="117">
+      <c r="D131" s="107">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="117" t="s">
+      <c r="A132" s="107" t="s">
         <v>193</v>
       </c>
-      <c r="B132" s="117">
+      <c r="B132" s="107">
         <f>STDEVA(TRUE,3,5)</f>
         <v>2</v>
       </c>
-      <c r="C132" s="117">
+      <c r="C132" s="107">
         <v>2</v>
       </c>
-      <c r="D132" s="117">
+      <c r="D132" s="107">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="117" t="s">
+      <c r="A133" s="107" t="s">
         <v>194</v>
       </c>
-      <c r="B133" s="117">
+      <c r="B133" s="107">
         <f>ROUND(STDEVP(2,5,8),2)</f>
         <v>2.4500000000000002</v>
       </c>
-      <c r="C133" s="117">
+      <c r="C133" s="107">
         <v>2.4500000000000002</v>
       </c>
-      <c r="D133" s="117">
+      <c r="D133" s="107">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="117" t="s">
+      <c r="A134" s="107" t="s">
         <v>195</v>
       </c>
-      <c r="B134" s="117">
+      <c r="B134" s="107">
         <f>ROUND(STDEVPA(TRUE,4,7),2)</f>
         <v>2.4500000000000002</v>
       </c>
-      <c r="C134" s="117">
+      <c r="C134" s="107">
         <v>2.4500000000000002</v>
       </c>
-      <c r="D134" s="117">
+      <c r="D134" s="107">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="117" t="s">
+      <c r="A135" s="107" t="s">
         <v>196</v>
       </c>
-      <c r="B135" s="117" t="str">
+      <c r="B135" s="107" t="str">
         <f>SUBSTITUTE("SAP is best","SAP","Odoo")</f>
         <v>Odoo is best</v>
       </c>
-      <c r="C135" s="117" t="s">
+      <c r="C135" s="107" t="s">
         <v>197</v>
       </c>
-      <c r="D135" s="117">
+      <c r="D135" s="107">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="117" t="s">
+      <c r="A136" s="107" t="s">
         <v>198</v>
       </c>
-      <c r="B136" s="117">
+      <c r="B136" s="107">
         <f>SUM(1,2,3,4,5)</f>
         <v>15</v>
       </c>
-      <c r="C136" s="117">
+      <c r="C136" s="107">
         <v>15</v>
       </c>
-      <c r="D136" s="117">
+      <c r="D136" s="107">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A137" s="117" t="s">
+      <c r="A137" s="107" t="s">
         <v>199</v>
       </c>
-      <c r="B137" s="117">
+      <c r="B137" s="107">
         <f>SUMIF(K2:K9,"&lt;100")</f>
         <v>52</v>
       </c>
-      <c r="C137" s="117">
+      <c r="C137" s="107">
         <v>52</v>
       </c>
-      <c r="D137" s="117">
+      <c r="D137" s="107">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="117" t="s">
+      <c r="A138" s="107" t="s">
         <v>200</v>
       </c>
-      <c r="B138" s="117">
+      <c r="B138" s="107">
         <f>SUMIFS(H2:H9,K2:K9,"&lt;100")</f>
         <v>201</v>
       </c>
-      <c r="C138" s="117">
+      <c r="C138" s="107">
         <v>201</v>
       </c>
-      <c r="D138" s="117">
+      <c r="D138" s="107">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A139" s="117" t="s">
+      <c r="A139" s="107" t="s">
         <v>201</v>
       </c>
-      <c r="B139" s="117">
+      <c r="B139" s="107">
         <f>ROUND(TAN(PI()/4),5)</f>
         <v>1</v>
       </c>
-      <c r="C139" s="117">
-        <v>1</v>
-      </c>
-      <c r="D139" s="117">
+      <c r="C139" s="107">
+        <v>1</v>
+      </c>
+      <c r="D139" s="107">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A140" s="117" t="s">
+      <c r="A140" s="107" t="s">
         <v>202</v>
       </c>
-      <c r="B140" s="117">
+      <c r="B140" s="107">
         <f>ROUND(TANH(1),5)</f>
         <v>0.76158999999999999</v>
       </c>
-      <c r="C140" s="117">
+      <c r="C140" s="107">
         <v>0.76158999999999999</v>
       </c>
-      <c r="D140" s="117">
+      <c r="D140" s="107">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A141" s="117" t="s">
+      <c r="A141" s="107" t="s">
         <v>203</v>
       </c>
-      <c r="B141" s="117" t="str">
+      <c r="B141" s="107" t="str">
         <f>_xlfn.TEXTJOIN("-",TRUE,"","1","A","%")</f>
         <v>1-A-%</v>
       </c>
-      <c r="C141" s="117" t="s">
+      <c r="C141" s="107" t="s">
         <v>204</v>
       </c>
-      <c r="D141" s="117">
+      <c r="D141" s="107">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A142" s="117" t="s">
+      <c r="A142" s="107" t="s">
         <v>205</v>
       </c>
       <c r="B142" s="20">
@@ -11779,235 +11743,235 @@
       <c r="C142" s="20">
         <v>0.38299768519999999</v>
       </c>
-      <c r="D142" s="117">
+      <c r="D142" s="107">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="117" t="s">
+      <c r="A143" s="107" t="s">
         <v>206</v>
       </c>
-      <c r="B143" s="117">
+      <c r="B143" s="107">
         <f>TIMEVALUE("18:00:00")</f>
         <v>0.75</v>
       </c>
-      <c r="C143" s="117">
+      <c r="C143" s="107">
         <v>0.75</v>
       </c>
-      <c r="D143" s="117">
+      <c r="D143" s="107">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A144" s="117" t="s">
+      <c r="A144" s="107" t="s">
         <v>207</v>
       </c>
       <c r="B144" s="18">
         <f ca="1">TODAY()</f>
         <v>45903</v>
       </c>
-      <c r="D144" s="117">
+      <c r="D144" s="107">
         <f ca="1">IF(ISNUMBER(B144),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="117" t="s">
+      <c r="A145" s="107" t="s">
         <v>208</v>
       </c>
-      <c r="B145" s="117" t="str">
+      <c r="B145" s="107" t="str">
         <f>TRIM(" Jean Ticonstitutionnalise ")</f>
         <v>Jean Ticonstitutionnalise</v>
       </c>
-      <c r="C145" s="117" t="s">
+      <c r="C145" s="107" t="s">
         <v>209</v>
       </c>
-      <c r="D145" s="117">
+      <c r="D145" s="107">
         <f t="shared" ref="D145:D163" si="9">IF(B145=C145,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A146" s="117" t="s">
+      <c r="A146" s="107" t="s">
         <v>210</v>
       </c>
-      <c r="B146" s="117">
+      <c r="B146" s="107">
         <f>TRUNC(42.42,1)</f>
         <v>42.4</v>
       </c>
-      <c r="C146" s="117">
+      <c r="C146" s="107">
         <v>42.4</v>
       </c>
-      <c r="D146" s="117">
+      <c r="D146" s="107">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A147" s="117" t="s">
+      <c r="A147" s="107" t="s">
         <v>211</v>
       </c>
-      <c r="B147" s="117" t="str">
+      <c r="B147" s="107" t="str">
         <f>UPPER("grrrr !")</f>
         <v>GRRRR !</v>
       </c>
-      <c r="C147" s="117" t="s">
+      <c r="C147" s="107" t="s">
         <v>212</v>
       </c>
-      <c r="D147" s="117">
+      <c r="D147" s="107">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A148" s="117" t="s">
+      <c r="A148" s="107" t="s">
         <v>213</v>
       </c>
-      <c r="B148" s="117">
+      <c r="B148" s="107">
         <f>ROUND(VAR(K1:K5),5)</f>
         <v>2.9166699999999999</v>
       </c>
-      <c r="C148" s="117">
+      <c r="C148" s="107">
         <v>2.9166699999999999</v>
       </c>
-      <c r="D148" s="117">
+      <c r="D148" s="107">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A149" s="117" t="s">
+      <c r="A149" s="107" t="s">
         <v>214</v>
       </c>
-      <c r="B149" s="117">
+      <c r="B149" s="107">
         <f>ROUND(_xlfn.VAR.P(K1:K5),5)</f>
         <v>2.1875</v>
       </c>
-      <c r="C149" s="117">
+      <c r="C149" s="107">
         <v>2.1875</v>
       </c>
-      <c r="D149" s="117">
+      <c r="D149" s="107">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A150" s="117" t="s">
+      <c r="A150" s="107" t="s">
         <v>215</v>
       </c>
-      <c r="B150" s="117">
+      <c r="B150" s="107">
         <f>_xlfn.VAR.S(2,5,8)</f>
         <v>9</v>
       </c>
-      <c r="C150" s="117">
+      <c r="C150" s="107">
         <v>9</v>
       </c>
-      <c r="D150" s="117">
+      <c r="D150" s="107">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A151" s="117" t="s">
+      <c r="A151" s="107" t="s">
         <v>216</v>
       </c>
-      <c r="B151" s="117">
+      <c r="B151" s="107">
         <f>ROUND(VARA(K1:K5),5)</f>
         <v>6.7</v>
       </c>
-      <c r="C151" s="117">
+      <c r="C151" s="107">
         <v>6.7</v>
       </c>
-      <c r="D151" s="117">
+      <c r="D151" s="107">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A152" s="117" t="s">
+      <c r="A152" s="107" t="s">
         <v>217</v>
       </c>
-      <c r="B152" s="117">
+      <c r="B152" s="107">
         <f>ROUND(VARP(K1:K5),5)</f>
         <v>2.1875</v>
       </c>
-      <c r="C152" s="117">
+      <c r="C152" s="107">
         <v>2.1875</v>
       </c>
-      <c r="D152" s="117">
+      <c r="D152" s="107">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A153" s="117" t="s">
+      <c r="A153" s="107" t="s">
         <v>218</v>
       </c>
-      <c r="B153" s="117">
+      <c r="B153" s="107">
         <f>ROUND(VARPA(K1:K5),5)</f>
         <v>5.36</v>
       </c>
-      <c r="C153" s="117">
+      <c r="C153" s="107">
         <v>5.36</v>
       </c>
-      <c r="D153" s="117">
+      <c r="D153" s="107">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A154" s="117" t="s">
+      <c r="A154" s="107" t="s">
         <v>219</v>
       </c>
-      <c r="B154" s="117">
+      <c r="B154" s="107">
         <f>VLOOKUP("NotACheater",G1:K9,3,FALSE)</f>
         <v>252.4</v>
       </c>
-      <c r="C154" s="117">
+      <c r="C154" s="107">
         <f>252.4</f>
         <v>252.4</v>
       </c>
-      <c r="D154" s="117">
+      <c r="D154" s="107">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A155" s="117" t="s">
+      <c r="A155" s="107" t="s">
         <v>220</v>
       </c>
-      <c r="B155" s="117">
+      <c r="B155" s="107">
         <f>WEEKDAY("2021-06-12")</f>
         <v>7</v>
       </c>
-      <c r="C155" s="117">
+      <c r="C155" s="107">
         <v>7</v>
       </c>
-      <c r="D155" s="117">
+      <c r="D155" s="107">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
     <row r="156" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A156" s="117" t="s">
+      <c r="A156" s="107" t="s">
         <v>221</v>
       </c>
-      <c r="B156" s="117">
+      <c r="B156" s="107">
         <f>WEEKNUM("2021-06-29")</f>
         <v>27</v>
       </c>
-      <c r="C156" s="117">
+      <c r="C156" s="107">
         <v>27</v>
       </c>
-      <c r="D156" s="117">
+      <c r="D156" s="107">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A157" s="117" t="s">
+      <c r="A157" s="107" t="s">
         <v>222</v>
       </c>
       <c r="B157" s="18">
@@ -12017,13 +11981,13 @@
       <c r="C157" s="18">
         <v>44278</v>
       </c>
-      <c r="D157" s="117">
+      <c r="D157" s="107">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A158" s="117" t="s">
+      <c r="A158" s="107" t="s">
         <v>223</v>
       </c>
       <c r="B158" s="18">
@@ -12033,87 +11997,87 @@
       <c r="C158" s="18">
         <v>44312</v>
       </c>
-      <c r="D158" s="117">
+      <c r="D158" s="107">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A159" s="117" t="s">
+      <c r="A159" s="107" t="s">
         <v>224</v>
       </c>
-      <c r="B159" s="117" t="b">
+      <c r="B159" s="107" t="b">
         <f>_xlfn.XOR(FALSE,TRUE,FALSE,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="C159" s="117" t="b">
-        <v>1</v>
-      </c>
-      <c r="D159" s="117">
+      <c r="C159" s="107" t="b">
+        <v>1</v>
+      </c>
+      <c r="D159" s="107">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
     <row r="160" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A160" s="117" t="s">
+      <c r="A160" s="107" t="s">
         <v>225</v>
       </c>
-      <c r="B160" s="117">
+      <c r="B160" s="107">
         <f>YEAR("2012-03-12")</f>
         <v>2012</v>
       </c>
-      <c r="C160" s="117">
+      <c r="C160" s="107">
         <v>2012</v>
       </c>
-      <c r="D160" s="117">
+      <c r="D160" s="107">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A161" s="117" t="s">
+      <c r="A161" s="107" t="s">
         <v>226</v>
       </c>
-      <c r="B161" s="117">
+      <c r="B161" s="107">
         <f>DELTA(1,1)</f>
         <v>1</v>
       </c>
-      <c r="C161" s="117">
-        <v>1</v>
-      </c>
-      <c r="D161" s="117">
+      <c r="C161" s="107">
+        <v>1</v>
+      </c>
+      <c r="D161" s="107">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
     <row r="162" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A162" s="117" t="s">
+      <c r="A162" s="107" t="s">
         <v>227</v>
       </c>
-      <c r="B162" s="117" t="str">
+      <c r="B162" s="107" t="str">
         <f>ADDRESS(1,1,4,FALSE,"sheet!")</f>
         <v>'sheet!'!R[1]C[1]</v>
       </c>
-      <c r="C162" s="117" t="s">
+      <c r="C162" s="107" t="s">
         <v>228</v>
       </c>
-      <c r="D162" s="117">
+      <c r="D162" s="107">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
     <row r="163" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A163" s="117" t="s">
+      <c r="A163" s="107" t="s">
         <v>229</v>
       </c>
-      <c r="B163" s="117">
+      <c r="B163" s="107">
         <f>DATEDIF("2002/01/01","2002/01/02","D")</f>
         <v>1</v>
       </c>
-      <c r="C163" s="117">
-        <v>1</v>
-      </c>
-      <c r="D163" s="117">
+      <c r="C163" s="107">
+        <v>1</v>
+      </c>
+      <c r="D163" s="107">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
@@ -12160,10 +12124,10 @@
       <c r="C1" t="s">
         <v>231</v>
       </c>
-      <c r="D1" s="123" t="s">
+      <c r="D1" s="113" t="s">
         <v>232</v>
       </c>
-      <c r="E1" s="123"/>
+      <c r="E1" s="113"/>
       <c r="F1" t="s">
         <v>233</v>
       </c>
@@ -12176,8 +12140,8 @@
         <f>SUM(A1)</f>
         <v>0</v>
       </c>
-      <c r="D2" s="123"/>
-      <c r="E2" s="123"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
       <c r="H2" t="str">
         <f>[1]Feuil1!$A$1</f>
         <v>referenced string</v>
@@ -12618,7 +12582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D919E811-4385-4D35-A19E-3B7E0E659A89}">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
@@ -13524,11 +13488,17 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B29:C29">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
+      <formula>$B$23</formula>
+      <formula>2+2</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B7:D7">
-    <cfRule type="duplicateValues" dxfId="2" priority="83"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="83"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:D14">
-    <cfRule type="uniqueValues" dxfId="1" priority="97"/>
+    <cfRule type="uniqueValues" dxfId="0" priority="97"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:J2">
     <cfRule type="colorScale" priority="45">
@@ -13785,12 +13755,6 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29:C29">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
-      <formula>$B$23</formula>
-      <formula>2+2</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
@@ -14006,96 +13970,96 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C4" s="117" t="s">
+      <c r="C4" s="107" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="117">
+      <c r="D4" s="107">
         <v>26</v>
       </c>
-      <c r="E4" s="117">
+      <c r="E4" s="107">
         <v>5</v>
       </c>
-      <c r="F4" s="117">
+      <c r="F4" s="107">
         <f>Table3[[#This Row],[Rank]]+Table3[[#This Row],[Age]]</f>
         <v>31</v>
       </c>
-      <c r="G4" s="117">
+      <c r="G4" s="107">
         <f>SUM(Table3[Rank])</f>
         <v>12</v>
       </c>
-      <c r="H4" s="117">
+      <c r="H4" s="107">
         <f>SUM(Table3[[#All],[Rank]])</f>
         <v>24</v>
       </c>
-      <c r="I4" s="117">
+      <c r="I4" s="107">
         <f>Table3[[#Totals],[Rank]]</f>
         <v>12</v>
       </c>
-      <c r="J4" s="117" t="str">
+      <c r="J4" s="107" t="str">
         <f>Table3[[#Headers],[Rank]]</f>
         <v>Rank</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C5" s="117" t="s">
+      <c r="C5" s="107" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="117">
+      <c r="D5" s="107">
         <v>13</v>
       </c>
-      <c r="E5" s="117">
+      <c r="E5" s="107">
         <v>7</v>
       </c>
-      <c r="F5" s="117">
+      <c r="F5" s="107">
         <f>Table3[[#This Row],[Rank]]+Table3[[#This Row],[Age]]</f>
         <v>20</v>
       </c>
-      <c r="G5" s="117">
+      <c r="G5" s="107">
         <f>SUM(Table3[Rank])</f>
         <v>12</v>
       </c>
-      <c r="H5" s="117">
+      <c r="H5" s="107">
         <f>SUM(Table3[[#All],[Rank]])</f>
         <v>24</v>
       </c>
-      <c r="I5" s="117">
+      <c r="I5" s="107">
         <f>Table3[[#Totals],[Rank]]</f>
         <v>12</v>
       </c>
-      <c r="J5" s="117" t="str">
+      <c r="J5" s="107" t="str">
         <f>Table3[[#Headers],[Rank]]</f>
         <v>Rank</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C6" s="117" t="s">
+      <c r="C6" s="107" t="s">
         <v>391</v>
       </c>
-      <c r="D6" s="117">
+      <c r="D6" s="107">
         <f>SUBTOTAL(109,Table3[Age])</f>
         <v>39</v>
       </c>
-      <c r="E6" s="117">
+      <c r="E6" s="107">
         <f>SUBTOTAL(109,Table3[Rank])</f>
         <v>12</v>
       </c>
-      <c r="F6" s="117">
+      <c r="F6" s="107">
         <f>SUBTOTAL(109,Table3[Rank+Age =E4+D4])</f>
         <v>51</v>
       </c>
-      <c r="G6" s="117">
+      <c r="G6" s="107">
         <f>SUBTOTAL(109,Table3[Data =SUM(E4:E5)])</f>
         <v>24</v>
       </c>
-      <c r="H6" s="117">
+      <c r="H6" s="107">
         <f>SUBTOTAL(109,Table3[All =SUM(E3:E6)])</f>
         <v>48</v>
       </c>
-      <c r="I6" s="117">
+      <c r="I6" s="107">
         <f>SUBTOTAL(109,Table3[Totals =E6])</f>
         <v>24</v>
       </c>
-      <c r="J6" s="117">
+      <c r="J6" s="107">
         <f>SUBTOTAL(109,Table3[Headers =E3])</f>
         <v>0</v>
       </c>
@@ -14366,16 +14330,16 @@
       <c r="F1" s="17"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="117"/>
-      <c r="B2" s="117"/>
-      <c r="C2" s="117"/>
-      <c r="D2" s="117"/>
-      <c r="E2" s="117"/>
-      <c r="F2" s="117"/>
+      <c r="A2" s="107"/>
+      <c r="B2" s="107"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="107"/>
+      <c r="F2" s="107"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="117"/>
-      <c r="B3" s="117"/>
+      <c r="A3" s="107"/>
+      <c r="B3" s="107"/>
       <c r="C3" s="89" t="s">
         <v>413</v>
       </c>
@@ -14384,8 +14348,8 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="117"/>
-      <c r="B4" s="117"/>
+      <c r="A4" s="107"/>
+      <c r="B4" s="107"/>
       <c r="C4" s="89" t="s">
         <v>415</v>
       </c>
@@ -14418,8 +14382,8 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="117"/>
-      <c r="B5" s="117"/>
+      <c r="A5" s="107"/>
+      <c r="B5" s="107"/>
       <c r="C5" s="90" t="s">
         <v>55</v>
       </c>
@@ -14431,8 +14395,8 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="117"/>
-      <c r="B6" s="117"/>
+      <c r="A6" s="107"/>
+      <c r="B6" s="107"/>
       <c r="C6" s="91">
         <v>256018</v>
       </c>
@@ -14444,8 +14408,8 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="117"/>
-      <c r="B7" s="117"/>
+      <c r="A7" s="107"/>
+      <c r="B7" s="107"/>
       <c r="C7" s="90" t="s">
         <v>46</v>
       </c>
@@ -14457,8 +14421,8 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="117"/>
-      <c r="B8" s="117"/>
+      <c r="A8" s="107"/>
+      <c r="B8" s="107"/>
       <c r="C8" s="91">
         <v>110120.5</v>
       </c>
@@ -14470,8 +14434,8 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="117"/>
-      <c r="B9" s="117"/>
+      <c r="A9" s="107"/>
+      <c r="B9" s="107"/>
       <c r="C9" s="90" t="s">
         <v>42</v>
       </c>
@@ -14483,8 +14447,8 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="117"/>
-      <c r="B10" s="117"/>
+      <c r="A10" s="107"/>
+      <c r="B10" s="107"/>
       <c r="C10" s="91">
         <v>25618</v>
       </c>
@@ -14666,7 +14630,7 @@
       <c r="A2" t="s">
         <v>418</v>
       </c>
-      <c r="B2" s="117"/>
+      <c r="B2" s="107"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">

</xml_diff>